<commit_message>
Mudando a lingugem para portugues dos cenarios
</commit_message>
<xml_diff>
--- a/target/Dados.xlsx
+++ b/target/Dados.xlsx
@@ -3,15 +3,19 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{B42CA694-9D70-47A3-BA0C-BADE5326ACFA}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joice.abreu\br.com.Rsinet.Hub.BDD\target\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{573BB980-5742-4B12-B012-57F31FF03FAC}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="2340" windowWidth="20655" windowHeight="11820" xr2:uid="{3811DB8B-1056-40F0-864D-B037B3637F44}"/>
+    <workbookView xWindow="0" yWindow="2505" windowWidth="20490" windowHeight="7875" xr2:uid="{3811DB8B-1056-40F0-864D-B037B3637F44}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -21,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>joice</t>
   </si>
@@ -105,6 +109,9 @@
   </si>
   <si>
     <t>JoiceGGG</t>
+  </si>
+  <si>
+    <t>JOOCEAA</t>
   </si>
 </sst>
 </file>
@@ -144,7 +151,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -196,11 +203,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -216,6 +234,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -530,10 +549,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0791D461-9D5A-4BBE-8A4B-109CA855029A}">
-  <dimension ref="A1:M4"/>
+  <dimension ref="A1:M5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -644,6 +663,11 @@
         <v>27</v>
       </c>
     </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" s="11" t="s">
+        <v>28</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>